<commit_message>
achei os melhores valores pra gerar os graficos
</commit_message>
<xml_diff>
--- a/resultados.xlsx
+++ b/resultados.xlsx
@@ -14,7 +14,7 @@
     <sheet name="Merge Sort" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Quick Sort" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Radix Sort" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Gráfico" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Gráfico Geral" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -144,6 +144,186 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10325100" cy="6677025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10315575" cy="6677025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10191750" cy="6677025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10191750" cy="6677025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10191750" cy="6677025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <oneCellAnchor>
+    <from>
+      <col>4</col>
+      <colOff>0</colOff>
+      <row>1</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="10067925" cy="6677025"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="1" name="Image 1" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+</wsDr>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
@@ -462,7 +642,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C127"/>
+  <dimension ref="A1:C121"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,10 +687,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="4">
@@ -520,10 +700,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>1914</v>
+        <v>7544</v>
       </c>
     </row>
     <row r="5">
@@ -533,10 +713,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>7566</v>
+        <v>16965</v>
       </c>
     </row>
     <row r="6">
@@ -546,10 +726,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>151</v>
+        <v>201</v>
       </c>
       <c r="C6" t="n">
-        <v>16962</v>
+        <v>30159</v>
       </c>
     </row>
     <row r="7">
@@ -559,10 +739,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="C7" t="n">
-        <v>30093</v>
+        <v>46984</v>
       </c>
     </row>
     <row r="8">
@@ -572,10 +752,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C8" t="n">
-        <v>46883</v>
+        <v>67758</v>
       </c>
     </row>
     <row r="9">
@@ -585,10 +765,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C9" t="n">
-        <v>67741</v>
+        <v>92224</v>
       </c>
     </row>
     <row r="10">
@@ -598,10 +778,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="C10" t="n">
-        <v>92067</v>
+        <v>120348</v>
       </c>
     </row>
     <row r="11">
@@ -611,10 +791,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="C11" t="n">
-        <v>120365</v>
+        <v>152609</v>
       </c>
     </row>
     <row r="12">
@@ -624,10 +804,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>451</v>
+        <v>501</v>
       </c>
       <c r="C12" t="n">
-        <v>152725</v>
+        <v>187372</v>
       </c>
     </row>
     <row r="13">
@@ -637,10 +817,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="C13" t="n">
-        <v>187810</v>
+        <v>227302</v>
       </c>
     </row>
     <row r="14">
@@ -650,10 +830,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>551</v>
+        <v>601</v>
       </c>
       <c r="C14" t="n">
-        <v>226462</v>
+        <v>270385</v>
       </c>
     </row>
     <row r="15">
@@ -663,10 +843,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>601</v>
+        <v>651</v>
       </c>
       <c r="C15" t="n">
-        <v>270496</v>
+        <v>316983</v>
       </c>
     </row>
     <row r="16">
@@ -676,10 +856,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="C16" t="n">
-        <v>316828</v>
+        <v>367528</v>
       </c>
     </row>
     <row r="17">
@@ -689,10 +869,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>701</v>
+        <v>751</v>
       </c>
       <c r="C17" t="n">
-        <v>368276</v>
+        <v>422499</v>
       </c>
     </row>
     <row r="18">
@@ -702,10 +882,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>751</v>
+        <v>801</v>
       </c>
       <c r="C18" t="n">
-        <v>422859</v>
+        <v>480323</v>
       </c>
     </row>
     <row r="19">
@@ -715,10 +895,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C19" t="n">
-        <v>481555</v>
+        <v>542782</v>
       </c>
     </row>
     <row r="20">
@@ -728,10 +908,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>851</v>
+        <v>901</v>
       </c>
       <c r="C20" t="n">
-        <v>541275</v>
+        <v>609269</v>
       </c>
     </row>
     <row r="21">
@@ -741,23 +921,23 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>901</v>
+        <v>951</v>
       </c>
       <c r="C21" t="n">
-        <v>606893</v>
+        <v>677870</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Bubble Sort</t>
+          <t>Insertion Sort</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>951</v>
+        <v>1</v>
       </c>
       <c r="C22" t="n">
-        <v>677717</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -767,10 +947,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="24">
@@ -780,10 +960,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>5188</v>
       </c>
     </row>
     <row r="25">
@@ -793,10 +973,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>51</v>
+        <v>151</v>
       </c>
       <c r="C25" t="n">
-        <v>1321</v>
+        <v>11482</v>
       </c>
     </row>
     <row r="26">
@@ -806,10 +986,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="C26" t="n">
-        <v>5182</v>
+        <v>20242</v>
       </c>
     </row>
     <row r="27">
@@ -819,10 +999,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>151</v>
+        <v>251</v>
       </c>
       <c r="C27" t="n">
-        <v>11426</v>
+        <v>31649</v>
       </c>
     </row>
     <row r="28">
@@ -832,10 +1012,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>201</v>
+        <v>301</v>
       </c>
       <c r="C28" t="n">
-        <v>20672</v>
+        <v>45660</v>
       </c>
     </row>
     <row r="29">
@@ -845,10 +1025,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>251</v>
+        <v>351</v>
       </c>
       <c r="C29" t="n">
-        <v>31416</v>
+        <v>62134</v>
       </c>
     </row>
     <row r="30">
@@ -858,10 +1038,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>301</v>
+        <v>401</v>
       </c>
       <c r="C30" t="n">
-        <v>45264</v>
+        <v>80812</v>
       </c>
     </row>
     <row r="31">
@@ -871,10 +1051,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>351</v>
+        <v>451</v>
       </c>
       <c r="C31" t="n">
-        <v>61689</v>
+        <v>101461</v>
       </c>
     </row>
     <row r="32">
@@ -884,10 +1064,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>401</v>
+        <v>501</v>
       </c>
       <c r="C32" t="n">
-        <v>81097</v>
+        <v>125203</v>
       </c>
     </row>
     <row r="33">
@@ -897,10 +1077,10 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>451</v>
+        <v>551</v>
       </c>
       <c r="C33" t="n">
-        <v>101541</v>
+        <v>151291</v>
       </c>
     </row>
     <row r="34">
@@ -910,10 +1090,10 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>501</v>
+        <v>601</v>
       </c>
       <c r="C34" t="n">
-        <v>126333</v>
+        <v>180835</v>
       </c>
     </row>
     <row r="35">
@@ -923,10 +1103,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>551</v>
+        <v>651</v>
       </c>
       <c r="C35" t="n">
-        <v>152420</v>
+        <v>213162</v>
       </c>
     </row>
     <row r="36">
@@ -936,10 +1116,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>601</v>
+        <v>701</v>
       </c>
       <c r="C36" t="n">
-        <v>181701</v>
+        <v>246682</v>
       </c>
     </row>
     <row r="37">
@@ -949,10 +1129,10 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>651</v>
+        <v>751</v>
       </c>
       <c r="C37" t="n">
-        <v>212372</v>
+        <v>284095</v>
       </c>
     </row>
     <row r="38">
@@ -962,10 +1142,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>701</v>
+        <v>801</v>
       </c>
       <c r="C38" t="n">
-        <v>246044</v>
+        <v>321666</v>
       </c>
     </row>
     <row r="39">
@@ -975,10 +1155,10 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>751</v>
+        <v>851</v>
       </c>
       <c r="C39" t="n">
-        <v>282639</v>
+        <v>365163</v>
       </c>
     </row>
     <row r="40">
@@ -988,10 +1168,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>801</v>
+        <v>901</v>
       </c>
       <c r="C40" t="n">
-        <v>321752</v>
+        <v>405613</v>
       </c>
     </row>
     <row r="41">
@@ -1001,36 +1181,36 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>851</v>
+        <v>951</v>
       </c>
       <c r="C41" t="n">
-        <v>362954</v>
+        <v>453023</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Insertion Sort</t>
+          <t>Heap Sort</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>901</v>
+        <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>403719</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Insertion Sort</t>
+          <t>Heap Sort</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>951</v>
+        <v>51</v>
       </c>
       <c r="C43" t="n">
-        <v>454987</v>
+        <v>670</v>
       </c>
     </row>
     <row r="44">
@@ -1040,10 +1220,10 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>1</v>
+        <v>101</v>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="45">
@@ -1053,10 +1233,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>1</v>
+        <v>151</v>
       </c>
       <c r="C45" t="n">
-        <v>0</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="46">
@@ -1066,10 +1246,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>51</v>
+        <v>201</v>
       </c>
       <c r="C46" t="n">
-        <v>671</v>
+        <v>3833</v>
       </c>
     </row>
     <row r="47">
@@ -1079,10 +1259,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>101</v>
+        <v>251</v>
       </c>
       <c r="C47" t="n">
-        <v>1632</v>
+        <v>5012</v>
       </c>
     </row>
     <row r="48">
@@ -1092,10 +1272,10 @@
         </is>
       </c>
       <c r="B48" t="n">
-        <v>151</v>
+        <v>301</v>
       </c>
       <c r="C48" t="n">
-        <v>2693</v>
+        <v>6266</v>
       </c>
     </row>
     <row r="49">
@@ -1105,10 +1285,10 @@
         </is>
       </c>
       <c r="B49" t="n">
-        <v>201</v>
+        <v>351</v>
       </c>
       <c r="C49" t="n">
-        <v>3844</v>
+        <v>7540</v>
       </c>
     </row>
     <row r="50">
@@ -1118,10 +1298,10 @@
         </is>
       </c>
       <c r="B50" t="n">
-        <v>251</v>
+        <v>401</v>
       </c>
       <c r="C50" t="n">
-        <v>5005</v>
+        <v>8853</v>
       </c>
     </row>
     <row r="51">
@@ -1131,10 +1311,10 @@
         </is>
       </c>
       <c r="B51" t="n">
-        <v>301</v>
+        <v>451</v>
       </c>
       <c r="C51" t="n">
-        <v>6253</v>
+        <v>10169</v>
       </c>
     </row>
     <row r="52">
@@ -1144,10 +1324,10 @@
         </is>
       </c>
       <c r="B52" t="n">
-        <v>351</v>
+        <v>501</v>
       </c>
       <c r="C52" t="n">
-        <v>7551</v>
+        <v>11513</v>
       </c>
     </row>
     <row r="53">
@@ -1157,10 +1337,10 @@
         </is>
       </c>
       <c r="B53" t="n">
-        <v>401</v>
+        <v>551</v>
       </c>
       <c r="C53" t="n">
-        <v>8848</v>
+        <v>12879</v>
       </c>
     </row>
     <row r="54">
@@ -1170,10 +1350,10 @@
         </is>
       </c>
       <c r="B54" t="n">
-        <v>451</v>
+        <v>601</v>
       </c>
       <c r="C54" t="n">
-        <v>10174</v>
+        <v>14303</v>
       </c>
     </row>
     <row r="55">
@@ -1183,10 +1363,10 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>501</v>
+        <v>651</v>
       </c>
       <c r="C55" t="n">
-        <v>11496</v>
+        <v>15722</v>
       </c>
     </row>
     <row r="56">
@@ -1196,10 +1376,10 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>551</v>
+        <v>701</v>
       </c>
       <c r="C56" t="n">
-        <v>12881</v>
+        <v>17158</v>
       </c>
     </row>
     <row r="57">
@@ -1209,10 +1389,10 @@
         </is>
       </c>
       <c r="B57" t="n">
-        <v>601</v>
+        <v>751</v>
       </c>
       <c r="C57" t="n">
-        <v>14295</v>
+        <v>18617</v>
       </c>
     </row>
     <row r="58">
@@ -1222,10 +1402,10 @@
         </is>
       </c>
       <c r="B58" t="n">
-        <v>651</v>
+        <v>801</v>
       </c>
       <c r="C58" t="n">
-        <v>15726</v>
+        <v>20069</v>
       </c>
     </row>
     <row r="59">
@@ -1235,10 +1415,10 @@
         </is>
       </c>
       <c r="B59" t="n">
-        <v>701</v>
+        <v>851</v>
       </c>
       <c r="C59" t="n">
-        <v>17167</v>
+        <v>21532</v>
       </c>
     </row>
     <row r="60">
@@ -1248,10 +1428,10 @@
         </is>
       </c>
       <c r="B60" t="n">
-        <v>751</v>
+        <v>901</v>
       </c>
       <c r="C60" t="n">
-        <v>18611</v>
+        <v>22991</v>
       </c>
     </row>
     <row r="61">
@@ -1261,49 +1441,49 @@
         </is>
       </c>
       <c r="B61" t="n">
-        <v>801</v>
+        <v>951</v>
       </c>
       <c r="C61" t="n">
-        <v>20068</v>
+        <v>24478</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Heap Sort</t>
+          <t>Merge Sort</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>851</v>
+        <v>1</v>
       </c>
       <c r="C62" t="n">
-        <v>21527</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Heap Sort</t>
+          <t>Merge Sort</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>901</v>
+        <v>51</v>
       </c>
       <c r="C63" t="n">
-        <v>23018</v>
+        <v>520</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Heap Sort</t>
+          <t>Merge Sort</t>
         </is>
       </c>
       <c r="B64" t="n">
-        <v>951</v>
+        <v>101</v>
       </c>
       <c r="C64" t="n">
-        <v>24489</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="65">
@@ -1313,10 +1493,10 @@
         </is>
       </c>
       <c r="B65" t="n">
-        <v>1</v>
+        <v>151</v>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="66">
@@ -1326,10 +1506,10 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="C66" t="n">
-        <v>0</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="67">
@@ -1339,10 +1519,10 @@
         </is>
       </c>
       <c r="B67" t="n">
-        <v>51</v>
+        <v>251</v>
       </c>
       <c r="C67" t="n">
-        <v>520</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="68">
@@ -1352,10 +1532,10 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>101</v>
+        <v>301</v>
       </c>
       <c r="C68" t="n">
-        <v>1228</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="69">
@@ -1365,10 +1545,10 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>151</v>
+        <v>351</v>
       </c>
       <c r="C69" t="n">
-        <v>2008</v>
+        <v>5533</v>
       </c>
     </row>
     <row r="70">
@@ -1378,10 +1558,10 @@
         </is>
       </c>
       <c r="B70" t="n">
-        <v>201</v>
+        <v>401</v>
       </c>
       <c r="C70" t="n">
-        <v>2843</v>
+        <v>6468</v>
       </c>
     </row>
     <row r="71">
@@ -1391,10 +1571,10 @@
         </is>
       </c>
       <c r="B71" t="n">
-        <v>251</v>
+        <v>451</v>
       </c>
       <c r="C71" t="n">
-        <v>3690</v>
+        <v>7415</v>
       </c>
     </row>
     <row r="72">
@@ -1404,10 +1584,10 @@
         </is>
       </c>
       <c r="B72" t="n">
-        <v>301</v>
+        <v>501</v>
       </c>
       <c r="C72" t="n">
-        <v>4605</v>
+        <v>8360</v>
       </c>
     </row>
     <row r="73">
@@ -1417,10 +1597,10 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>351</v>
+        <v>551</v>
       </c>
       <c r="C73" t="n">
-        <v>5534</v>
+        <v>9366</v>
       </c>
     </row>
     <row r="74">
@@ -1430,10 +1610,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>401</v>
+        <v>601</v>
       </c>
       <c r="C74" t="n">
-        <v>6466</v>
+        <v>10387</v>
       </c>
     </row>
     <row r="75">
@@ -1443,10 +1623,10 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>451</v>
+        <v>651</v>
       </c>
       <c r="C75" t="n">
-        <v>7418</v>
+        <v>11413</v>
       </c>
     </row>
     <row r="76">
@@ -1456,10 +1636,10 @@
         </is>
       </c>
       <c r="B76" t="n">
-        <v>501</v>
+        <v>701</v>
       </c>
       <c r="C76" t="n">
-        <v>8360</v>
+        <v>12445</v>
       </c>
     </row>
     <row r="77">
@@ -1469,10 +1649,10 @@
         </is>
       </c>
       <c r="B77" t="n">
-        <v>551</v>
+        <v>751</v>
       </c>
       <c r="C77" t="n">
-        <v>9368</v>
+        <v>13478</v>
       </c>
     </row>
     <row r="78">
@@ -1482,10 +1662,10 @@
         </is>
       </c>
       <c r="B78" t="n">
-        <v>601</v>
+        <v>801</v>
       </c>
       <c r="C78" t="n">
-        <v>10388</v>
+        <v>14522</v>
       </c>
     </row>
     <row r="79">
@@ -1495,10 +1675,10 @@
         </is>
       </c>
       <c r="B79" t="n">
-        <v>651</v>
+        <v>851</v>
       </c>
       <c r="C79" t="n">
-        <v>11415</v>
+        <v>15565</v>
       </c>
     </row>
     <row r="80">
@@ -1508,10 +1688,10 @@
         </is>
       </c>
       <c r="B80" t="n">
-        <v>701</v>
+        <v>901</v>
       </c>
       <c r="C80" t="n">
-        <v>12439</v>
+        <v>16600</v>
       </c>
     </row>
     <row r="81">
@@ -1521,62 +1701,62 @@
         </is>
       </c>
       <c r="B81" t="n">
-        <v>751</v>
+        <v>951</v>
       </c>
       <c r="C81" t="n">
-        <v>13473</v>
+        <v>17651</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Merge Sort</t>
+          <t>Quick Sort</t>
         </is>
       </c>
       <c r="B82" t="n">
-        <v>801</v>
+        <v>1</v>
       </c>
       <c r="C82" t="n">
-        <v>14521</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Merge Sort</t>
+          <t>Quick Sort</t>
         </is>
       </c>
       <c r="B83" t="n">
-        <v>851</v>
+        <v>51</v>
       </c>
       <c r="C83" t="n">
-        <v>15561</v>
+        <v>429</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Merge Sort</t>
+          <t>Quick Sort</t>
         </is>
       </c>
       <c r="B84" t="n">
-        <v>901</v>
+        <v>101</v>
       </c>
       <c r="C84" t="n">
-        <v>16605</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Merge Sort</t>
+          <t>Quick Sort</t>
         </is>
       </c>
       <c r="B85" t="n">
-        <v>951</v>
+        <v>151</v>
       </c>
       <c r="C85" t="n">
-        <v>17659</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="86">
@@ -1586,10 +1766,10 @@
         </is>
       </c>
       <c r="B86" t="n">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="87">
@@ -1599,10 +1779,10 @@
         </is>
       </c>
       <c r="B87" t="n">
-        <v>1</v>
+        <v>251</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="88">
@@ -1612,10 +1792,10 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>51</v>
+        <v>301</v>
       </c>
       <c r="C88" t="n">
-        <v>437</v>
+        <v>4082</v>
       </c>
     </row>
     <row r="89">
@@ -1625,10 +1805,10 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>101</v>
+        <v>351</v>
       </c>
       <c r="C89" t="n">
-        <v>1047</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="90">
@@ -1638,10 +1818,10 @@
         </is>
       </c>
       <c r="B90" t="n">
-        <v>151</v>
+        <v>401</v>
       </c>
       <c r="C90" t="n">
-        <v>1759</v>
+        <v>5753</v>
       </c>
     </row>
     <row r="91">
@@ -1651,10 +1831,10 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>201</v>
+        <v>451</v>
       </c>
       <c r="C91" t="n">
-        <v>2444</v>
+        <v>6829</v>
       </c>
     </row>
     <row r="92">
@@ -1664,10 +1844,10 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>251</v>
+        <v>501</v>
       </c>
       <c r="C92" t="n">
-        <v>3305</v>
+        <v>7773</v>
       </c>
     </row>
     <row r="93">
@@ -1677,10 +1857,10 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>301</v>
+        <v>551</v>
       </c>
       <c r="C93" t="n">
-        <v>4042</v>
+        <v>8468</v>
       </c>
     </row>
     <row r="94">
@@ -1690,10 +1870,10 @@
         </is>
       </c>
       <c r="B94" t="n">
-        <v>351</v>
+        <v>601</v>
       </c>
       <c r="C94" t="n">
-        <v>4940</v>
+        <v>9341</v>
       </c>
     </row>
     <row r="95">
@@ -1703,10 +1883,10 @@
         </is>
       </c>
       <c r="B95" t="n">
-        <v>401</v>
+        <v>651</v>
       </c>
       <c r="C95" t="n">
-        <v>5790</v>
+        <v>10546</v>
       </c>
     </row>
     <row r="96">
@@ -1716,10 +1896,10 @@
         </is>
       </c>
       <c r="B96" t="n">
-        <v>451</v>
+        <v>701</v>
       </c>
       <c r="C96" t="n">
-        <v>6743</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="97">
@@ -1729,10 +1909,10 @@
         </is>
       </c>
       <c r="B97" t="n">
-        <v>501</v>
+        <v>751</v>
       </c>
       <c r="C97" t="n">
-        <v>7463</v>
+        <v>12291</v>
       </c>
     </row>
     <row r="98">
@@ -1742,10 +1922,10 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>551</v>
+        <v>801</v>
       </c>
       <c r="C98" t="n">
-        <v>8516</v>
+        <v>13391</v>
       </c>
     </row>
     <row r="99">
@@ -1755,10 +1935,10 @@
         </is>
       </c>
       <c r="B99" t="n">
-        <v>601</v>
+        <v>851</v>
       </c>
       <c r="C99" t="n">
-        <v>9627</v>
+        <v>13946</v>
       </c>
     </row>
     <row r="100">
@@ -1768,10 +1948,10 @@
         </is>
       </c>
       <c r="B100" t="n">
-        <v>651</v>
+        <v>901</v>
       </c>
       <c r="C100" t="n">
-        <v>10311</v>
+        <v>15101</v>
       </c>
     </row>
     <row r="101">
@@ -1781,75 +1961,75 @@
         </is>
       </c>
       <c r="B101" t="n">
-        <v>701</v>
+        <v>951</v>
       </c>
       <c r="C101" t="n">
-        <v>11372</v>
+        <v>16016</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Quick Sort</t>
+          <t>Radix Sort</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>751</v>
+        <v>1</v>
       </c>
       <c r="C102" t="n">
-        <v>12187</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Quick Sort</t>
+          <t>Radix Sort</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>801</v>
+        <v>51</v>
       </c>
       <c r="C103" t="n">
-        <v>13027</v>
+        <v>254</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Quick Sort</t>
+          <t>Radix Sort</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>851</v>
+        <v>101</v>
       </c>
       <c r="C104" t="n">
-        <v>14348</v>
+        <v>504</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Quick Sort</t>
+          <t>Radix Sort</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>901</v>
+        <v>151</v>
       </c>
       <c r="C105" t="n">
-        <v>14949</v>
+        <v>754</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Quick Sort</t>
+          <t>Radix Sort</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>951</v>
+        <v>201</v>
       </c>
       <c r="C106" t="n">
-        <v>16223</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="107">
@@ -1859,10 +2039,10 @@
         </is>
       </c>
       <c r="B107" t="n">
-        <v>1</v>
+        <v>251</v>
       </c>
       <c r="C107" t="n">
-        <v>3</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="108">
@@ -1872,10 +2052,10 @@
         </is>
       </c>
       <c r="B108" t="n">
-        <v>1</v>
+        <v>301</v>
       </c>
       <c r="C108" t="n">
-        <v>3</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="109">
@@ -1885,10 +2065,10 @@
         </is>
       </c>
       <c r="B109" t="n">
-        <v>51</v>
+        <v>351</v>
       </c>
       <c r="C109" t="n">
-        <v>254</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="110">
@@ -1898,10 +2078,10 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>101</v>
+        <v>401</v>
       </c>
       <c r="C110" t="n">
-        <v>504</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="111">
@@ -1911,10 +2091,10 @@
         </is>
       </c>
       <c r="B111" t="n">
-        <v>151</v>
+        <v>451</v>
       </c>
       <c r="C111" t="n">
-        <v>754</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="112">
@@ -1924,10 +2104,10 @@
         </is>
       </c>
       <c r="B112" t="n">
-        <v>201</v>
+        <v>501</v>
       </c>
       <c r="C112" t="n">
-        <v>1004</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="113">
@@ -1937,10 +2117,10 @@
         </is>
       </c>
       <c r="B113" t="n">
-        <v>251</v>
+        <v>551</v>
       </c>
       <c r="C113" t="n">
-        <v>1254</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="114">
@@ -1950,10 +2130,10 @@
         </is>
       </c>
       <c r="B114" t="n">
-        <v>301</v>
+        <v>601</v>
       </c>
       <c r="C114" t="n">
-        <v>1504</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="115">
@@ -1963,10 +2143,10 @@
         </is>
       </c>
       <c r="B115" t="n">
-        <v>351</v>
+        <v>651</v>
       </c>
       <c r="C115" t="n">
-        <v>1754</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="116">
@@ -1976,10 +2156,10 @@
         </is>
       </c>
       <c r="B116" t="n">
-        <v>401</v>
+        <v>701</v>
       </c>
       <c r="C116" t="n">
-        <v>2004</v>
+        <v>3504</v>
       </c>
     </row>
     <row r="117">
@@ -1989,10 +2169,10 @@
         </is>
       </c>
       <c r="B117" t="n">
-        <v>451</v>
+        <v>751</v>
       </c>
       <c r="C117" t="n">
-        <v>2254</v>
+        <v>3754</v>
       </c>
     </row>
     <row r="118">
@@ -2002,10 +2182,10 @@
         </is>
       </c>
       <c r="B118" t="n">
-        <v>501</v>
+        <v>801</v>
       </c>
       <c r="C118" t="n">
-        <v>2504</v>
+        <v>4004</v>
       </c>
     </row>
     <row r="119">
@@ -2015,10 +2195,10 @@
         </is>
       </c>
       <c r="B119" t="n">
-        <v>551</v>
+        <v>851</v>
       </c>
       <c r="C119" t="n">
-        <v>2754</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="120">
@@ -2028,10 +2208,10 @@
         </is>
       </c>
       <c r="B120" t="n">
-        <v>601</v>
+        <v>901</v>
       </c>
       <c r="C120" t="n">
-        <v>3004</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="121">
@@ -2041,87 +2221,9 @@
         </is>
       </c>
       <c r="B121" t="n">
-        <v>651</v>
+        <v>951</v>
       </c>
       <c r="C121" t="n">
-        <v>3254</v>
-      </c>
-    </row>
-    <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>Radix Sort</t>
-        </is>
-      </c>
-      <c r="B122" t="n">
-        <v>701</v>
-      </c>
-      <c r="C122" t="n">
-        <v>3504</v>
-      </c>
-    </row>
-    <row r="123">
-      <c r="A123" t="inlineStr">
-        <is>
-          <t>Radix Sort</t>
-        </is>
-      </c>
-      <c r="B123" t="n">
-        <v>751</v>
-      </c>
-      <c r="C123" t="n">
-        <v>3754</v>
-      </c>
-    </row>
-    <row r="124">
-      <c r="A124" t="inlineStr">
-        <is>
-          <t>Radix Sort</t>
-        </is>
-      </c>
-      <c r="B124" t="n">
-        <v>801</v>
-      </c>
-      <c r="C124" t="n">
-        <v>4004</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>Radix Sort</t>
-        </is>
-      </c>
-      <c r="B125" t="n">
-        <v>851</v>
-      </c>
-      <c r="C125" t="n">
-        <v>4254</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>Radix Sort</t>
-        </is>
-      </c>
-      <c r="B126" t="n">
-        <v>901</v>
-      </c>
-      <c r="C126" t="n">
-        <v>4504</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>Radix Sort</t>
-        </is>
-      </c>
-      <c r="B127" t="n">
-        <v>951</v>
-      </c>
-      <c r="C127" t="n">
         <v>4754</v>
       </c>
     </row>
@@ -2136,7 +2238,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2181,10 +2283,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="4">
@@ -2194,10 +2296,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>1914</v>
+        <v>7544</v>
       </c>
     </row>
     <row r="5">
@@ -2207,10 +2309,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>7566</v>
+        <v>16965</v>
       </c>
     </row>
     <row r="6">
@@ -2220,10 +2322,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>151</v>
+        <v>201</v>
       </c>
       <c r="C6" t="n">
-        <v>16962</v>
+        <v>30159</v>
       </c>
     </row>
     <row r="7">
@@ -2233,10 +2335,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="C7" t="n">
-        <v>30093</v>
+        <v>46984</v>
       </c>
     </row>
     <row r="8">
@@ -2246,10 +2348,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C8" t="n">
-        <v>46883</v>
+        <v>67758</v>
       </c>
     </row>
     <row r="9">
@@ -2259,10 +2361,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C9" t="n">
-        <v>67741</v>
+        <v>92224</v>
       </c>
     </row>
     <row r="10">
@@ -2272,10 +2374,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="C10" t="n">
-        <v>92067</v>
+        <v>120348</v>
       </c>
     </row>
     <row r="11">
@@ -2285,10 +2387,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="C11" t="n">
-        <v>120365</v>
+        <v>152609</v>
       </c>
     </row>
     <row r="12">
@@ -2298,10 +2400,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>451</v>
+        <v>501</v>
       </c>
       <c r="C12" t="n">
-        <v>152725</v>
+        <v>187372</v>
       </c>
     </row>
     <row r="13">
@@ -2311,10 +2413,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="C13" t="n">
-        <v>187810</v>
+        <v>227302</v>
       </c>
     </row>
     <row r="14">
@@ -2324,10 +2426,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>551</v>
+        <v>601</v>
       </c>
       <c r="C14" t="n">
-        <v>226462</v>
+        <v>270385</v>
       </c>
     </row>
     <row r="15">
@@ -2337,10 +2439,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>601</v>
+        <v>651</v>
       </c>
       <c r="C15" t="n">
-        <v>270496</v>
+        <v>316983</v>
       </c>
     </row>
     <row r="16">
@@ -2350,10 +2452,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="C16" t="n">
-        <v>316828</v>
+        <v>367528</v>
       </c>
     </row>
     <row r="17">
@@ -2363,10 +2465,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>701</v>
+        <v>751</v>
       </c>
       <c r="C17" t="n">
-        <v>368276</v>
+        <v>422499</v>
       </c>
     </row>
     <row r="18">
@@ -2376,10 +2478,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>751</v>
+        <v>801</v>
       </c>
       <c r="C18" t="n">
-        <v>422859</v>
+        <v>480323</v>
       </c>
     </row>
     <row r="19">
@@ -2389,10 +2491,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C19" t="n">
-        <v>481555</v>
+        <v>542782</v>
       </c>
     </row>
     <row r="20">
@@ -2402,10 +2504,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>851</v>
+        <v>901</v>
       </c>
       <c r="C20" t="n">
-        <v>541275</v>
+        <v>609269</v>
       </c>
     </row>
     <row r="21">
@@ -2415,27 +2517,15 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>901</v>
+        <v>951</v>
       </c>
       <c r="C21" t="n">
-        <v>606893</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Bubble Sort</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>951</v>
-      </c>
-      <c r="C22" t="n">
-        <v>677717</v>
+        <v>677870</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2445,7 +2535,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2490,10 +2580,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="4">
@@ -2503,10 +2593,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>1321</v>
+        <v>5188</v>
       </c>
     </row>
     <row r="5">
@@ -2516,10 +2606,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>5182</v>
+        <v>11482</v>
       </c>
     </row>
     <row r="6">
@@ -2529,10 +2619,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>151</v>
+        <v>201</v>
       </c>
       <c r="C6" t="n">
-        <v>11426</v>
+        <v>20242</v>
       </c>
     </row>
     <row r="7">
@@ -2542,10 +2632,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="C7" t="n">
-        <v>20672</v>
+        <v>31649</v>
       </c>
     </row>
     <row r="8">
@@ -2555,10 +2645,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C8" t="n">
-        <v>31416</v>
+        <v>45660</v>
       </c>
     </row>
     <row r="9">
@@ -2568,10 +2658,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C9" t="n">
-        <v>45264</v>
+        <v>62134</v>
       </c>
     </row>
     <row r="10">
@@ -2581,10 +2671,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="C10" t="n">
-        <v>61689</v>
+        <v>80812</v>
       </c>
     </row>
     <row r="11">
@@ -2594,10 +2684,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="C11" t="n">
-        <v>81097</v>
+        <v>101461</v>
       </c>
     </row>
     <row r="12">
@@ -2607,10 +2697,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>451</v>
+        <v>501</v>
       </c>
       <c r="C12" t="n">
-        <v>101541</v>
+        <v>125203</v>
       </c>
     </row>
     <row r="13">
@@ -2620,10 +2710,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="C13" t="n">
-        <v>126333</v>
+        <v>151291</v>
       </c>
     </row>
     <row r="14">
@@ -2633,10 +2723,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>551</v>
+        <v>601</v>
       </c>
       <c r="C14" t="n">
-        <v>152420</v>
+        <v>180835</v>
       </c>
     </row>
     <row r="15">
@@ -2646,10 +2736,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>601</v>
+        <v>651</v>
       </c>
       <c r="C15" t="n">
-        <v>181701</v>
+        <v>213162</v>
       </c>
     </row>
     <row r="16">
@@ -2659,10 +2749,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="C16" t="n">
-        <v>212372</v>
+        <v>246682</v>
       </c>
     </row>
     <row r="17">
@@ -2672,10 +2762,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>701</v>
+        <v>751</v>
       </c>
       <c r="C17" t="n">
-        <v>246044</v>
+        <v>284095</v>
       </c>
     </row>
     <row r="18">
@@ -2685,10 +2775,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>751</v>
+        <v>801</v>
       </c>
       <c r="C18" t="n">
-        <v>282639</v>
+        <v>321666</v>
       </c>
     </row>
     <row r="19">
@@ -2698,10 +2788,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C19" t="n">
-        <v>321752</v>
+        <v>365163</v>
       </c>
     </row>
     <row r="20">
@@ -2711,10 +2801,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>851</v>
+        <v>901</v>
       </c>
       <c r="C20" t="n">
-        <v>362954</v>
+        <v>405613</v>
       </c>
     </row>
     <row r="21">
@@ -2724,27 +2814,15 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>901</v>
+        <v>951</v>
       </c>
       <c r="C21" t="n">
-        <v>403719</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Insertion Sort</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>951</v>
-      </c>
-      <c r="C22" t="n">
-        <v>454987</v>
+        <v>453023</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2754,7 +2832,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2799,10 +2877,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>670</v>
       </c>
     </row>
     <row r="4">
@@ -2812,10 +2890,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>671</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="5">
@@ -2825,10 +2903,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>1632</v>
+        <v>2697</v>
       </c>
     </row>
     <row r="6">
@@ -2838,10 +2916,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>151</v>
+        <v>201</v>
       </c>
       <c r="C6" t="n">
-        <v>2693</v>
+        <v>3833</v>
       </c>
     </row>
     <row r="7">
@@ -2851,10 +2929,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="C7" t="n">
-        <v>3844</v>
+        <v>5012</v>
       </c>
     </row>
     <row r="8">
@@ -2864,10 +2942,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C8" t="n">
-        <v>5005</v>
+        <v>6266</v>
       </c>
     </row>
     <row r="9">
@@ -2877,10 +2955,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C9" t="n">
-        <v>6253</v>
+        <v>7540</v>
       </c>
     </row>
     <row r="10">
@@ -2890,10 +2968,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="C10" t="n">
-        <v>7551</v>
+        <v>8853</v>
       </c>
     </row>
     <row r="11">
@@ -2903,10 +2981,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="C11" t="n">
-        <v>8848</v>
+        <v>10169</v>
       </c>
     </row>
     <row r="12">
@@ -2916,10 +2994,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>451</v>
+        <v>501</v>
       </c>
       <c r="C12" t="n">
-        <v>10174</v>
+        <v>11513</v>
       </c>
     </row>
     <row r="13">
@@ -2929,10 +3007,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="C13" t="n">
-        <v>11496</v>
+        <v>12879</v>
       </c>
     </row>
     <row r="14">
@@ -2942,10 +3020,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>551</v>
+        <v>601</v>
       </c>
       <c r="C14" t="n">
-        <v>12881</v>
+        <v>14303</v>
       </c>
     </row>
     <row r="15">
@@ -2955,10 +3033,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>601</v>
+        <v>651</v>
       </c>
       <c r="C15" t="n">
-        <v>14295</v>
+        <v>15722</v>
       </c>
     </row>
     <row r="16">
@@ -2968,10 +3046,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="C16" t="n">
-        <v>15726</v>
+        <v>17158</v>
       </c>
     </row>
     <row r="17">
@@ -2981,10 +3059,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>701</v>
+        <v>751</v>
       </c>
       <c r="C17" t="n">
-        <v>17167</v>
+        <v>18617</v>
       </c>
     </row>
     <row r="18">
@@ -2994,10 +3072,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>751</v>
+        <v>801</v>
       </c>
       <c r="C18" t="n">
-        <v>18611</v>
+        <v>20069</v>
       </c>
     </row>
     <row r="19">
@@ -3007,10 +3085,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C19" t="n">
-        <v>20068</v>
+        <v>21532</v>
       </c>
     </row>
     <row r="20">
@@ -3020,10 +3098,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>851</v>
+        <v>901</v>
       </c>
       <c r="C20" t="n">
-        <v>21527</v>
+        <v>22991</v>
       </c>
     </row>
     <row r="21">
@@ -3033,27 +3111,15 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>901</v>
+        <v>951</v>
       </c>
       <c r="C21" t="n">
-        <v>23018</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Heap Sort</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>951</v>
-      </c>
-      <c r="C22" t="n">
-        <v>24489</v>
+        <v>24478</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3063,7 +3129,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3108,10 +3174,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>520</v>
       </c>
     </row>
     <row r="4">
@@ -3121,10 +3187,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>520</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="5">
@@ -3134,10 +3200,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>1228</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="6">
@@ -3147,10 +3213,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>151</v>
+        <v>201</v>
       </c>
       <c r="C6" t="n">
-        <v>2008</v>
+        <v>2842</v>
       </c>
     </row>
     <row r="7">
@@ -3160,10 +3226,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="C7" t="n">
-        <v>2843</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="8">
@@ -3173,10 +3239,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C8" t="n">
-        <v>3690</v>
+        <v>4603</v>
       </c>
     </row>
     <row r="9">
@@ -3186,10 +3252,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C9" t="n">
-        <v>4605</v>
+        <v>5533</v>
       </c>
     </row>
     <row r="10">
@@ -3199,10 +3265,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="C10" t="n">
-        <v>5534</v>
+        <v>6468</v>
       </c>
     </row>
     <row r="11">
@@ -3212,10 +3278,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="C11" t="n">
-        <v>6466</v>
+        <v>7415</v>
       </c>
     </row>
     <row r="12">
@@ -3225,10 +3291,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>451</v>
+        <v>501</v>
       </c>
       <c r="C12" t="n">
-        <v>7418</v>
+        <v>8360</v>
       </c>
     </row>
     <row r="13">
@@ -3238,10 +3304,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="C13" t="n">
-        <v>8360</v>
+        <v>9366</v>
       </c>
     </row>
     <row r="14">
@@ -3251,10 +3317,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>551</v>
+        <v>601</v>
       </c>
       <c r="C14" t="n">
-        <v>9368</v>
+        <v>10387</v>
       </c>
     </row>
     <row r="15">
@@ -3264,10 +3330,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>601</v>
+        <v>651</v>
       </c>
       <c r="C15" t="n">
-        <v>10388</v>
+        <v>11413</v>
       </c>
     </row>
     <row r="16">
@@ -3277,10 +3343,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="C16" t="n">
-        <v>11415</v>
+        <v>12445</v>
       </c>
     </row>
     <row r="17">
@@ -3290,10 +3356,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>701</v>
+        <v>751</v>
       </c>
       <c r="C17" t="n">
-        <v>12439</v>
+        <v>13478</v>
       </c>
     </row>
     <row r="18">
@@ -3303,10 +3369,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>751</v>
+        <v>801</v>
       </c>
       <c r="C18" t="n">
-        <v>13473</v>
+        <v>14522</v>
       </c>
     </row>
     <row r="19">
@@ -3316,10 +3382,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C19" t="n">
-        <v>14521</v>
+        <v>15565</v>
       </c>
     </row>
     <row r="20">
@@ -3329,10 +3395,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>851</v>
+        <v>901</v>
       </c>
       <c r="C20" t="n">
-        <v>15561</v>
+        <v>16600</v>
       </c>
     </row>
     <row r="21">
@@ -3342,27 +3408,15 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>901</v>
+        <v>951</v>
       </c>
       <c r="C21" t="n">
-        <v>16605</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Merge Sort</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>951</v>
-      </c>
-      <c r="C22" t="n">
-        <v>17659</v>
+        <v>17651</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3372,7 +3426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3417,10 +3471,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4">
@@ -3430,10 +3484,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>437</v>
+        <v>1051</v>
       </c>
     </row>
     <row r="5">
@@ -3443,10 +3497,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>1047</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="6">
@@ -3456,10 +3510,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>151</v>
+        <v>201</v>
       </c>
       <c r="C6" t="n">
-        <v>1759</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="7">
@@ -3469,10 +3523,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="C7" t="n">
-        <v>2444</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="8">
@@ -3482,10 +3536,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C8" t="n">
-        <v>3305</v>
+        <v>4082</v>
       </c>
     </row>
     <row r="9">
@@ -3495,10 +3549,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C9" t="n">
-        <v>4042</v>
+        <v>4971</v>
       </c>
     </row>
     <row r="10">
@@ -3508,10 +3562,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="C10" t="n">
-        <v>4940</v>
+        <v>5753</v>
       </c>
     </row>
     <row r="11">
@@ -3521,10 +3575,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="C11" t="n">
-        <v>5790</v>
+        <v>6829</v>
       </c>
     </row>
     <row r="12">
@@ -3534,10 +3588,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>451</v>
+        <v>501</v>
       </c>
       <c r="C12" t="n">
-        <v>6743</v>
+        <v>7773</v>
       </c>
     </row>
     <row r="13">
@@ -3547,10 +3601,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="C13" t="n">
-        <v>7463</v>
+        <v>8468</v>
       </c>
     </row>
     <row r="14">
@@ -3560,10 +3614,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>551</v>
+        <v>601</v>
       </c>
       <c r="C14" t="n">
-        <v>8516</v>
+        <v>9341</v>
       </c>
     </row>
     <row r="15">
@@ -3573,10 +3627,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>601</v>
+        <v>651</v>
       </c>
       <c r="C15" t="n">
-        <v>9627</v>
+        <v>10546</v>
       </c>
     </row>
     <row r="16">
@@ -3586,10 +3640,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="C16" t="n">
-        <v>10311</v>
+        <v>11792</v>
       </c>
     </row>
     <row r="17">
@@ -3599,10 +3653,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>701</v>
+        <v>751</v>
       </c>
       <c r="C17" t="n">
-        <v>11372</v>
+        <v>12291</v>
       </c>
     </row>
     <row r="18">
@@ -3612,10 +3666,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>751</v>
+        <v>801</v>
       </c>
       <c r="C18" t="n">
-        <v>12187</v>
+        <v>13391</v>
       </c>
     </row>
     <row r="19">
@@ -3625,10 +3679,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C19" t="n">
-        <v>13027</v>
+        <v>13946</v>
       </c>
     </row>
     <row r="20">
@@ -3638,10 +3692,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>851</v>
+        <v>901</v>
       </c>
       <c r="C20" t="n">
-        <v>14348</v>
+        <v>15101</v>
       </c>
     </row>
     <row r="21">
@@ -3651,27 +3705,15 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>901</v>
+        <v>951</v>
       </c>
       <c r="C21" t="n">
-        <v>14949</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Quick Sort</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>951</v>
-      </c>
-      <c r="C22" t="n">
-        <v>16223</v>
+        <v>16016</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3681,7 +3723,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3726,10 +3768,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>51</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>254</v>
       </c>
     </row>
     <row r="4">
@@ -3739,10 +3781,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>51</v>
+        <v>101</v>
       </c>
       <c r="C4" t="n">
-        <v>254</v>
+        <v>504</v>
       </c>
     </row>
     <row r="5">
@@ -3752,10 +3794,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>101</v>
+        <v>151</v>
       </c>
       <c r="C5" t="n">
-        <v>504</v>
+        <v>754</v>
       </c>
     </row>
     <row r="6">
@@ -3765,10 +3807,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>151</v>
+        <v>201</v>
       </c>
       <c r="C6" t="n">
-        <v>754</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="7">
@@ -3778,10 +3820,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201</v>
+        <v>251</v>
       </c>
       <c r="C7" t="n">
-        <v>1004</v>
+        <v>1254</v>
       </c>
     </row>
     <row r="8">
@@ -3791,10 +3833,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>251</v>
+        <v>301</v>
       </c>
       <c r="C8" t="n">
-        <v>1254</v>
+        <v>1504</v>
       </c>
     </row>
     <row r="9">
@@ -3804,10 +3846,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C9" t="n">
-        <v>1504</v>
+        <v>1754</v>
       </c>
     </row>
     <row r="10">
@@ -3817,10 +3859,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>351</v>
+        <v>401</v>
       </c>
       <c r="C10" t="n">
-        <v>1754</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="11">
@@ -3830,10 +3872,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>401</v>
+        <v>451</v>
       </c>
       <c r="C11" t="n">
-        <v>2004</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="12">
@@ -3843,10 +3885,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>451</v>
+        <v>501</v>
       </c>
       <c r="C12" t="n">
-        <v>2254</v>
+        <v>2504</v>
       </c>
     </row>
     <row r="13">
@@ -3856,10 +3898,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>501</v>
+        <v>551</v>
       </c>
       <c r="C13" t="n">
-        <v>2504</v>
+        <v>2754</v>
       </c>
     </row>
     <row r="14">
@@ -3869,10 +3911,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>551</v>
+        <v>601</v>
       </c>
       <c r="C14" t="n">
-        <v>2754</v>
+        <v>3004</v>
       </c>
     </row>
     <row r="15">
@@ -3882,10 +3924,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>601</v>
+        <v>651</v>
       </c>
       <c r="C15" t="n">
-        <v>3004</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="16">
@@ -3895,10 +3937,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>651</v>
+        <v>701</v>
       </c>
       <c r="C16" t="n">
-        <v>3254</v>
+        <v>3504</v>
       </c>
     </row>
     <row r="17">
@@ -3908,10 +3950,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>701</v>
+        <v>751</v>
       </c>
       <c r="C17" t="n">
-        <v>3504</v>
+        <v>3754</v>
       </c>
     </row>
     <row r="18">
@@ -3921,10 +3963,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>751</v>
+        <v>801</v>
       </c>
       <c r="C18" t="n">
-        <v>3754</v>
+        <v>4004</v>
       </c>
     </row>
     <row r="19">
@@ -3934,10 +3976,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>801</v>
+        <v>851</v>
       </c>
       <c r="C19" t="n">
-        <v>4004</v>
+        <v>4254</v>
       </c>
     </row>
     <row r="20">
@@ -3947,10 +3989,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>851</v>
+        <v>901</v>
       </c>
       <c r="C20" t="n">
-        <v>4254</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="21">
@@ -3960,27 +4002,15 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>901</v>
+        <v>951</v>
       </c>
       <c r="C21" t="n">
-        <v>4504</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t>Radix Sort</t>
-        </is>
-      </c>
-      <c r="B22" t="n">
-        <v>951</v>
-      </c>
-      <c r="C22" t="n">
         <v>4754</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>